<commit_message>
An extra sheet was added to final dataset that contains the number of CUs, populations and streams in each region.
</commit_message>
<xml_diff>
--- a/data_output/populationAssessed_catches_data.xlsx
+++ b/data_output/populationAssessed_catches_data.xlsx
@@ -11,12 +11,13 @@
     <sheet name="populations_species" r:id="rId5" sheetId="3"/>
     <sheet name="populations_regions_species" r:id="rId6" sheetId="4"/>
     <sheet name="catches_species_total" r:id="rId7" sheetId="5"/>
+    <sheet name="summary_regions" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9167" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9211" uniqueCount="52">
   <si>
     <t>year</t>
   </si>
@@ -80,6 +81,99 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>CU_nb</t>
+  </si>
+  <si>
+    <t>pop_nb</t>
+  </si>
+  <si>
+    <t>site_nb</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>389</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>748</t>
+  </si>
+  <si>
+    <t>244</t>
+  </si>
+  <si>
+    <t>825</t>
+  </si>
+  <si>
+    <t>1657</t>
+  </si>
+  <si>
+    <t>2230</t>
+  </si>
+  <si>
+    <t>936</t>
+  </si>
+  <si>
+    <t>6766</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>423</t>
+  </si>
+  <si>
+    <t>660</t>
+  </si>
+  <si>
+    <t>577</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2393</t>
+  </si>
 </sst>
 </file>
 
@@ -102937,4 +103031,171 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>